<commit_message>
Fixed the padding problem. Added real 5D tests. The 5D demo referenced in the README.
</commit_message>
<xml_diff>
--- a/examples/multid-output.xlsx
+++ b/examples/multid-output.xlsx
@@ -19,10 +19,10 @@
     <t>{{ | data | header | 1:0 }}</t>
   </si>
   <si>
-    <t>{{ A2 | 1 * data | header | 0:1 }}</t>
-  </si>
-  <si>
-    <t>{{ C2 | data | header | 1:0 }}</t>
+    <t>{{ A2 | 1 * data | header | 1 }}</t>
+  </si>
+  <si>
+    <t>{{ C2 | data | header | 1 }}</t>
   </si>
   <si>
     <t>{{ B3 | data * data || 1:1 }}</t>
@@ -31,13 +31,19 @@
     <t xml:space="preserve">Dimension 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Dimension 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dimension 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dimension 4</t>
+    <t xml:space="preserve">Dimension 2 - 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension 3 - 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension 3 - 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension 3 - 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension 4 - 1</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.1.1.1</t>
@@ -310,6 +316,9 @@
     <t xml:space="preserve">1.3.1.5.6</t>
   </si>
   <si>
+    <t xml:space="preserve">Dimension 4 - 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.2.1.1</t>
   </si>
   <si>
@@ -580,6 +589,9 @@
     <t xml:space="preserve">1.3.2.5.6</t>
   </si>
   <si>
+    <t xml:space="preserve">Dimension 4 - 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.3.1.1</t>
   </si>
   <si>
@@ -850,6 +862,9 @@
     <t xml:space="preserve">1.3.3.5.6</t>
   </si>
   <si>
+    <t xml:space="preserve">Dimension 4 - 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.4.1.1</t>
   </si>
   <si>
@@ -1118,6 +1133,9 @@
   </si>
   <si>
     <t xml:space="preserve">1.3.4.5.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimension 2 - 2</t>
   </si>
   <si>
     <t xml:space="preserve">2.1.1.1.1</t>
@@ -3491,7 +3509,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="J2" t="s" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -3499,7 +3517,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="Q2" t="s" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
@@ -3511,307 +3529,307 @@
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E3" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s" s="5">
-        <v>8</v>
-      </c>
       <c r="J3" t="s" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O3" t="s" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q3" t="s" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R3" t="s" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S3" t="s" s="5">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="U3" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="V3" t="s" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" t="s" s="5">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s" s="5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s" s="5">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N4" t="s" s="5">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O4" t="s" s="5">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" t="s" s="5">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="R4" t="s" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s" s="5">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T4" t="s" s="5">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="U4" t="s" s="5">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="V4" t="s" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" t="s" s="5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s" s="5">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="5">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s" s="5">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O5" t="s" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" t="s" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R5" t="s" s="5">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S5" t="s" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T5" t="s" s="5">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="U5" t="s" s="5">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="V5" t="s" s="5">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" t="s" s="5">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s" s="5">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N6" t="s" s="5">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O6" t="s" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" t="s" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="R6" t="s" s="5">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="S6" t="s" s="5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="T6" t="s" s="5">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="U6" t="s" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="V6" t="s" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" t="s" s="5">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s" s="5">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s" s="5">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="5">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K7" t="s" s="5">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s" s="5">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N7" t="s" s="5">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="O7" t="s" s="5">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" t="s" s="5">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="R7" t="s" s="5">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="S7" t="s" s="5">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T7" t="s" s="5">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U7" t="s" s="5">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="V7" t="s" s="5">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
@@ -3825,307 +3843,307 @@
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" t="s" s="5">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s" s="5">
+        <v>104</v>
+      </c>
+      <c r="F9" t="s" s="5">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s" s="5">
+        <v>106</v>
+      </c>
+      <c r="H9" t="s" s="5">
+        <v>107</v>
+      </c>
+      <c r="I9" t="s" s="5">
         <v>101</v>
       </c>
-      <c r="F9" t="s" s="5">
-        <v>102</v>
-      </c>
-      <c r="G9" t="s" s="5">
-        <v>103</v>
-      </c>
-      <c r="H9" t="s" s="5">
-        <v>104</v>
-      </c>
-      <c r="I9" t="s" s="5">
-        <v>8</v>
-      </c>
       <c r="J9" t="s" s="5">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K9" t="s" s="5">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="L9" t="s" s="5">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N9" t="s" s="5">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O9" t="s" s="5">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="P9" t="s" s="5">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="Q9" t="s" s="5">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="R9" t="s" s="5">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="S9" t="s" s="5">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="T9" t="s" s="5">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="U9" t="s" s="5">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="V9" t="s" s="5">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" t="s" s="5">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s" s="5">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F10" t="s" s="5">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G10" t="s" s="5">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s" s="5">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K10" t="s" s="5">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="L10" t="s" s="5">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="N10" t="s" s="5">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="O10" t="s" s="5">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" t="s" s="5">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="R10" t="s" s="5">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="S10" t="s" s="5">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="T10" t="s" s="5">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="U10" t="s" s="5">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="V10" t="s" s="5">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" t="s" s="5">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s" s="5">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F11" t="s" s="5">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H11" t="s" s="5">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="5">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="K11" t="s" s="5">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="L11" t="s" s="5">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M11" t="s" s="5">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="N11" t="s" s="5">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="O11" t="s" s="5">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" t="s" s="5">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="R11" t="s" s="5">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="S11" t="s" s="5">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="T11" t="s" s="5">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="U11" t="s" s="5">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="V11" t="s" s="5">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" t="s" s="5">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s" s="5">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F12" t="s" s="5">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G12" t="s" s="5">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H12" t="s" s="5">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="5">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K12" t="s" s="5">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="L12" t="s" s="5">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="M12" t="s" s="5">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="N12" t="s" s="5">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="O12" t="s" s="5">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" t="s" s="5">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="R12" t="s" s="5">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="S12" t="s" s="5">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="T12" t="s" s="5">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="U12" t="s" s="5">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="V12" t="s" s="5">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" t="s" s="5">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E13" t="s" s="5">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F13" t="s" s="5">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G13" t="s" s="5">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H13" t="s" s="5">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="5">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="K13" t="s" s="5">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="L13" t="s" s="5">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M13" t="s" s="5">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="N13" t="s" s="5">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="O13" t="s" s="5">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" t="s" s="5">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="R13" t="s" s="5">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="S13" t="s" s="5">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="T13" t="s" s="5">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="U13" t="s" s="5">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="V13" t="s" s="5">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
@@ -4139,307 +4157,307 @@
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" t="s" s="5">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E15" t="s" s="5">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F15" t="s" s="5">
+        <v>196</v>
+      </c>
+      <c r="G15" t="s" s="5">
+        <v>197</v>
+      </c>
+      <c r="H15" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="I15" t="s" s="5">
         <v>192</v>
       </c>
-      <c r="G15" t="s" s="5">
-        <v>193</v>
-      </c>
-      <c r="H15" t="s" s="5">
-        <v>194</v>
-      </c>
-      <c r="I15" t="s" s="5">
-        <v>8</v>
-      </c>
       <c r="J15" t="s" s="5">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K15" t="s" s="5">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="L15" t="s" s="5">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M15" t="s" s="5">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="N15" t="s" s="5">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="O15" t="s" s="5">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="P15" t="s" s="5">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="Q15" t="s" s="5">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="R15" t="s" s="5">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="S15" t="s" s="5">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="T15" t="s" s="5">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="U15" t="s" s="5">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="V15" t="s" s="5">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" t="s" s="5">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s" s="5">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F16" t="s" s="5">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G16" t="s" s="5">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H16" t="s" s="5">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="5">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K16" t="s" s="5">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="L16" t="s" s="5">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="M16" t="s" s="5">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="N16" t="s" s="5">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="O16" t="s" s="5">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" t="s" s="5">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="R16" t="s" s="5">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="S16" t="s" s="5">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="T16" t="s" s="5">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="U16" t="s" s="5">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="V16" t="s" s="5">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" t="s" s="5">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E17" t="s" s="5">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F17" t="s" s="5">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G17" t="s" s="5">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H17" t="s" s="5">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="5">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="K17" t="s" s="5">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="L17" t="s" s="5">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="M17" t="s" s="5">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N17" t="s" s="5">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="O17" t="s" s="5">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" t="s" s="5">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="R17" t="s" s="5">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="S17" t="s" s="5">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="T17" t="s" s="5">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="U17" t="s" s="5">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="V17" t="s" s="5">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" t="s" s="5">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E18" t="s" s="5">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F18" t="s" s="5">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G18" t="s" s="5">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="H18" t="s" s="5">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="5">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="K18" t="s" s="5">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="L18" t="s" s="5">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="M18" t="s" s="5">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="N18" t="s" s="5">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="O18" t="s" s="5">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" t="s" s="5">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="R18" t="s" s="5">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="S18" t="s" s="5">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="T18" t="s" s="5">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="U18" t="s" s="5">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="V18" t="s" s="5">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" t="s" s="5">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E19" t="s" s="5">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F19" t="s" s="5">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="G19" t="s" s="5">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="H19" t="s" s="5">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="5">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K19" t="s" s="5">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="L19" t="s" s="5">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="M19" t="s" s="5">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="N19" t="s" s="5">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="O19" t="s" s="5">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" t="s" s="5">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="R19" t="s" s="5">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S19" t="s" s="5">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="T19" t="s" s="5">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U19" t="s" s="5">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V19" t="s" s="5">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
@@ -4453,312 +4471,312 @@
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" t="s" s="5">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="E21" t="s" s="5">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="F21" t="s" s="5">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="G21" t="s" s="5">
+        <v>288</v>
+      </c>
+      <c r="H21" t="s" s="5">
+        <v>289</v>
+      </c>
+      <c r="I21" t="s" s="5">
         <v>283</v>
       </c>
-      <c r="H21" t="s" s="5">
-        <v>284</v>
-      </c>
-      <c r="I21" t="s" s="5">
-        <v>8</v>
-      </c>
       <c r="J21" t="s" s="5">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="K21" t="s" s="5">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="L21" t="s" s="5">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="M21" t="s" s="5">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="N21" t="s" s="5">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="O21" t="s" s="5">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="P21" t="s" s="5">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="Q21" t="s" s="5">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="R21" t="s" s="5">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="S21" t="s" s="5">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="T21" t="s" s="5">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="U21" t="s" s="5">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="V21" t="s" s="5">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" t="s" s="5">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="E22" t="s" s="5">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="F22" t="s" s="5">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="G22" t="s" s="5">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="H22" t="s" s="5">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="5">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="K22" t="s" s="5">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="L22" t="s" s="5">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="M22" t="s" s="5">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="N22" t="s" s="5">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="O22" t="s" s="5">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" t="s" s="5">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="R22" t="s" s="5">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="S22" t="s" s="5">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="T22" t="s" s="5">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="U22" t="s" s="5">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="V22" t="s" s="5">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" t="s" s="5">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="D23" t="s" s="5">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="E23" t="s" s="5">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F23" t="s" s="5">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="G23" t="s" s="5">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H23" t="s" s="5">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" t="s" s="5">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="K23" t="s" s="5">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="L23" t="s" s="5">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="M23" t="s" s="5">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="N23" t="s" s="5">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="O23" t="s" s="5">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" t="s" s="5">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="R23" t="s" s="5">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="S23" t="s" s="5">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="T23" t="s" s="5">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U23" t="s" s="5">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="V23" t="s" s="5">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" t="s" s="5">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D24" t="s" s="5">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="E24" t="s" s="5">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F24" t="s" s="5">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="G24" t="s" s="5">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="H24" t="s" s="5">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" t="s" s="5">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="K24" t="s" s="5">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="L24" t="s" s="5">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="M24" t="s" s="5">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="N24" t="s" s="5">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="O24" t="s" s="5">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" t="s" s="5">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="R24" t="s" s="5">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="S24" t="s" s="5">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="T24" t="s" s="5">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="U24" t="s" s="5">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="V24" t="s" s="5">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" t="s" s="5">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="E25" t="s" s="5">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="F25" t="s" s="5">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G25" t="s" s="5">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="H25" t="s" s="5">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" t="s" s="5">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="K25" t="s" s="5">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="L25" t="s" s="5">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="M25" t="s" s="5">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="N25" t="s" s="5">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="O25" t="s" s="5">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" t="s" s="5">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="R25" t="s" s="5">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="S25" t="s" s="5">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="T25" t="s" s="5">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="U25" t="s" s="5">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="V25" t="s" s="5">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="5">
-        <v>6</v>
+        <v>374</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" t="s" s="5">
@@ -4771,7 +4789,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="1"/>
       <c r="J27" t="s" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -4780,7 +4798,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="1"/>
       <c r="Q27" t="s" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
@@ -4792,307 +4810,307 @@
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="D28" t="s" s="5">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="E28" t="s" s="5">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="F28" t="s" s="5">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="G28" t="s" s="5">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="H28" t="s" s="5">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="I28" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J28" t="s" s="5">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="K28" t="s" s="5">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="L28" t="s" s="5">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="M28" t="s" s="5">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="N28" t="s" s="5">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="O28" t="s" s="5">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="P28" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q28" t="s" s="5">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="R28" t="s" s="5">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="S28" t="s" s="5">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="T28" t="s" s="5">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="U28" t="s" s="5">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="V28" t="s" s="5">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" t="s" s="5">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="D29" t="s" s="5">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="E29" t="s" s="5">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="F29" t="s" s="5">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="G29" t="s" s="5">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="H29" t="s" s="5">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" t="s" s="5">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="K29" t="s" s="5">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="L29" t="s" s="5">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="M29" t="s" s="5">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="N29" t="s" s="5">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="O29" t="s" s="5">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" t="s" s="5">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="R29" t="s" s="5">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="S29" t="s" s="5">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="T29" t="s" s="5">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="U29" t="s" s="5">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="V29" t="s" s="5">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" t="s" s="5">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="D30" t="s" s="5">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="E30" t="s" s="5">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="F30" t="s" s="5">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="G30" t="s" s="5">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="H30" t="s" s="5">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" t="s" s="5">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="K30" t="s" s="5">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="L30" t="s" s="5">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="M30" t="s" s="5">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="N30" t="s" s="5">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="O30" t="s" s="5">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" t="s" s="5">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="R30" t="s" s="5">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="S30" t="s" s="5">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="T30" t="s" s="5">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="U30" t="s" s="5">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="V30" t="s" s="5">
-        <v>422</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" t="s" s="5">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E31" t="s" s="5">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="F31" t="s" s="5">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="G31" t="s" s="5">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="H31" t="s" s="5">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" t="s" s="5">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="K31" t="s" s="5">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="L31" t="s" s="5">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="M31" t="s" s="5">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="N31" t="s" s="5">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="O31" t="s" s="5">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" t="s" s="5">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="R31" t="s" s="5">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="S31" t="s" s="5">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="T31" t="s" s="5">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="U31" t="s" s="5">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="V31" t="s" s="5">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" t="s" s="5">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="D32" t="s" s="5">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="E32" t="s" s="5">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="F32" t="s" s="5">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="G32" t="s" s="5">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="H32" t="s" s="5">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" t="s" s="5">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="K32" t="s" s="5">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="L32" t="s" s="5">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="M32" t="s" s="5">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="N32" t="s" s="5">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="O32" t="s" s="5">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" t="s" s="5">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="R32" t="s" s="5">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="S32" t="s" s="5">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="T32" t="s" s="5">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="U32" t="s" s="5">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="V32" t="s" s="5">
-        <v>458</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
@@ -5101,307 +5119,307 @@
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" t="s" s="5">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s" s="5">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="D34" t="s" s="5">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="E34" t="s" s="5">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="F34" t="s" s="5">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="G34" t="s" s="5">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="H34" t="s" s="5">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="I34" t="s" s="5">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="J34" t="s" s="5">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="K34" t="s" s="5">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="L34" t="s" s="5">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="M34" t="s" s="5">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="N34" t="s" s="5">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="O34" t="s" s="5">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="P34" t="s" s="5">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="Q34" t="s" s="5">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="R34" t="s" s="5">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="S34" t="s" s="5">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="T34" t="s" s="5">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="U34" t="s" s="5">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="V34" t="s" s="5">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" t="s" s="5">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="D35" t="s" s="5">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="E35" t="s" s="5">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="F35" t="s" s="5">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="G35" t="s" s="5">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="H35" t="s" s="5">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" t="s" s="5">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="K35" t="s" s="5">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="L35" t="s" s="5">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="M35" t="s" s="5">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="N35" t="s" s="5">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="O35" t="s" s="5">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" t="s" s="5">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="R35" t="s" s="5">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="S35" t="s" s="5">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="T35" t="s" s="5">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="U35" t="s" s="5">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="V35" t="s" s="5">
-        <v>494</v>
+        <v>500</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" t="s" s="5">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="D36" t="s" s="5">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="E36" t="s" s="5">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="F36" t="s" s="5">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="G36" t="s" s="5">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="H36" t="s" s="5">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" t="s" s="5">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="K36" t="s" s="5">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="L36" t="s" s="5">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="M36" t="s" s="5">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="N36" t="s" s="5">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="O36" t="s" s="5">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="P36" s="5"/>
       <c r="Q36" t="s" s="5">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="R36" t="s" s="5">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="S36" t="s" s="5">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="T36" t="s" s="5">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="U36" t="s" s="5">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="V36" t="s" s="5">
-        <v>512</v>
+        <v>518</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" t="s" s="5">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="E37" t="s" s="5">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="F37" t="s" s="5">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="G37" t="s" s="5">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="H37" t="s" s="5">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" t="s" s="5">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="K37" t="s" s="5">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="L37" t="s" s="5">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="M37" t="s" s="5">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="N37" t="s" s="5">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="O37" t="s" s="5">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" t="s" s="5">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="R37" t="s" s="5">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="S37" t="s" s="5">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="T37" t="s" s="5">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="U37" t="s" s="5">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="V37" t="s" s="5">
-        <v>530</v>
+        <v>536</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" t="s" s="5">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="E38" t="s" s="5">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="F38" t="s" s="5">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="G38" t="s" s="5">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="H38" t="s" s="5">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" t="s" s="5">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="K38" t="s" s="5">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="L38" t="s" s="5">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="M38" t="s" s="5">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="N38" t="s" s="5">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="O38" t="s" s="5">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="P38" s="5"/>
       <c r="Q38" t="s" s="5">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="R38" t="s" s="5">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="S38" t="s" s="5">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="T38" t="s" s="5">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="U38" t="s" s="5">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="V38" t="s" s="5">
-        <v>548</v>
+        <v>554</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
@@ -5410,307 +5428,307 @@
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" t="s" s="5">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="E40" t="s" s="5">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="F40" t="s" s="5">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="G40" t="s" s="5">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="H40" t="s" s="5">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="I40" t="s" s="5">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="J40" t="s" s="5">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="K40" t="s" s="5">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="L40" t="s" s="5">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="M40" t="s" s="5">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="N40" t="s" s="5">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="O40" t="s" s="5">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="P40" t="s" s="5">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="Q40" t="s" s="5">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="R40" t="s" s="5">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="S40" t="s" s="5">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="T40" t="s" s="5">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="U40" t="s" s="5">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="V40" t="s" s="5">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" t="s" s="5">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="E41" t="s" s="5">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="F41" t="s" s="5">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="G41" t="s" s="5">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="H41" t="s" s="5">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" t="s" s="5">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="K41" t="s" s="5">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="L41" t="s" s="5">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="M41" t="s" s="5">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="N41" t="s" s="5">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="O41" t="s" s="5">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="P41" s="5"/>
       <c r="Q41" t="s" s="5">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="R41" t="s" s="5">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="S41" t="s" s="5">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="T41" t="s" s="5">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="U41" t="s" s="5">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="V41" t="s" s="5">
-        <v>584</v>
+        <v>590</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" t="s" s="5">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="E42" t="s" s="5">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="F42" t="s" s="5">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="G42" t="s" s="5">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="H42" t="s" s="5">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" t="s" s="5">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="K42" t="s" s="5">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="L42" t="s" s="5">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="M42" t="s" s="5">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="N42" t="s" s="5">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="O42" t="s" s="5">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" t="s" s="5">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="R42" t="s" s="5">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="S42" t="s" s="5">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="T42" t="s" s="5">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="U42" t="s" s="5">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="V42" t="s" s="5">
-        <v>602</v>
+        <v>608</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" t="s" s="5">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="E43" t="s" s="5">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="F43" t="s" s="5">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="G43" t="s" s="5">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="H43" t="s" s="5">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" t="s" s="5">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="K43" t="s" s="5">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="L43" t="s" s="5">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="M43" t="s" s="5">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="N43" t="s" s="5">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="O43" t="s" s="5">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" t="s" s="5">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="R43" t="s" s="5">
-        <v>616</v>
+        <v>622</v>
       </c>
       <c r="S43" t="s" s="5">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="T43" t="s" s="5">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="U43" t="s" s="5">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="V43" t="s" s="5">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" t="s" s="5">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>622</v>
+        <v>628</v>
       </c>
       <c r="E44" t="s" s="5">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="F44" t="s" s="5">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="G44" t="s" s="5">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="H44" t="s" s="5">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" t="s" s="5">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="K44" t="s" s="5">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="L44" t="s" s="5">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="M44" t="s" s="5">
-        <v>630</v>
+        <v>636</v>
       </c>
       <c r="N44" t="s" s="5">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="O44" t="s" s="5">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" t="s" s="5">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="R44" t="s" s="5">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="S44" t="s" s="5">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="T44" t="s" s="5">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="U44" t="s" s="5">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="V44" t="s" s="5">
-        <v>638</v>
+        <v>644</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
@@ -5719,307 +5737,307 @@
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" t="s" s="5">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="D46" t="s" s="5">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="E46" t="s" s="5">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="F46" t="s" s="5">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="G46" t="s" s="5">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="H46" t="s" s="5">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="I46" t="s" s="5">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="J46" t="s" s="5">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="K46" t="s" s="5">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="L46" t="s" s="5">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="M46" t="s" s="5">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="N46" t="s" s="5">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="O46" t="s" s="5">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="P46" t="s" s="5">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="Q46" t="s" s="5">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="R46" t="s" s="5">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="S46" t="s" s="5">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="T46" t="s" s="5">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="U46" t="s" s="5">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="V46" t="s" s="5">
-        <v>656</v>
+        <v>662</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" t="s" s="5">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="D47" t="s" s="5">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="E47" t="s" s="5">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="F47" t="s" s="5">
-        <v>660</v>
+        <v>666</v>
       </c>
       <c r="G47" t="s" s="5">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="H47" t="s" s="5">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" t="s" s="5">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="K47" t="s" s="5">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="L47" t="s" s="5">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="M47" t="s" s="5">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="N47" t="s" s="5">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="O47" t="s" s="5">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="P47" s="5"/>
       <c r="Q47" t="s" s="5">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="R47" t="s" s="5">
-        <v>670</v>
+        <v>676</v>
       </c>
       <c r="S47" t="s" s="5">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="T47" t="s" s="5">
-        <v>672</v>
+        <v>678</v>
       </c>
       <c r="U47" t="s" s="5">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="V47" t="s" s="5">
-        <v>674</v>
+        <v>680</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" t="s" s="5">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="E48" t="s" s="5">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="F48" t="s" s="5">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="G48" t="s" s="5">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="H48" t="s" s="5">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" t="s" s="5">
-        <v>681</v>
+        <v>687</v>
       </c>
       <c r="K48" t="s" s="5">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="L48" t="s" s="5">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="M48" t="s" s="5">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="N48" t="s" s="5">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="O48" t="s" s="5">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" t="s" s="5">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="R48" t="s" s="5">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c r="S48" t="s" s="5">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="T48" t="s" s="5">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="U48" t="s" s="5">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c r="V48" t="s" s="5">
-        <v>692</v>
+        <v>698</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" t="s" s="5">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>694</v>
+        <v>700</v>
       </c>
       <c r="E49" t="s" s="5">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="F49" t="s" s="5">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="G49" t="s" s="5">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="H49" t="s" s="5">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" t="s" s="5">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="K49" t="s" s="5">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="L49" t="s" s="5">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="M49" t="s" s="5">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="N49" t="s" s="5">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="O49" t="s" s="5">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" t="s" s="5">
-        <v>705</v>
+        <v>711</v>
       </c>
       <c r="R49" t="s" s="5">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="S49" t="s" s="5">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="T49" t="s" s="5">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="U49" t="s" s="5">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="V49" t="s" s="5">
-        <v>710</v>
+        <v>716</v>
       </c>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" t="s" s="5">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="D50" t="s" s="5">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="E50" t="s" s="5">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="F50" t="s" s="5">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c r="G50" t="s" s="5">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="H50" t="s" s="5">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" t="s" s="5">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="K50" t="s" s="5">
-        <v>718</v>
+        <v>724</v>
       </c>
       <c r="L50" t="s" s="5">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="M50" t="s" s="5">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="N50" t="s" s="5">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="O50" t="s" s="5">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="P50" s="5"/>
       <c r="Q50" t="s" s="5">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="R50" t="s" s="5">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="S50" t="s" s="5">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="T50" t="s" s="5">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="U50" t="s" s="5">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="V50" t="s" s="5">
-        <v>728</v>
+        <v>734</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
Add the ability to specify options clarifications on each cell, using the styling field.
</commit_message>
<xml_diff>
--- a/examples/multid-output.xlsx
+++ b/examples/multid-output.xlsx
@@ -6,6 +6,7 @@
   </bookViews>
   <sheets>
     <sheet name="5D" sheetId="1" r:id="rId4"/>
+    <sheet name="4D-merges" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -26,6 +27,15 @@
   </si>
   <si>
     <t>{{ B3 | data * data || 1:1 }}</t>
+  </si>
+  <si>
+    <t>{{ | data.1.data | header | 1:0 }}</t>
+  </si>
+  <si>
+    <t>{{ A2 | 1 * data | header | 1 | !mergeCells=false}}</t>
+  </si>
+  <si>
+    <t>{{ B2 | data * data || 1 }}</t>
   </si>
   <si>
     <t xml:space="preserve">Dimension 1</t>
@@ -2371,6 +2381,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3487,7 +3500,7 @@
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -3497,11 +3510,11 @@
     </row>
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" t="s" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3509,7 +3522,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="J2" t="s" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -3517,7 +3530,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="Q2" t="s" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
@@ -3529,307 +3542,307 @@
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="F3" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s" s="5">
-        <v>10</v>
-      </c>
       <c r="J3" t="s" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s" s="5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s" s="5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s" s="5">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s" s="5">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q3" t="s" s="5">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="R3" t="s" s="5">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S3" t="s" s="5">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s" s="5">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="U3" t="s" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="V3" t="s" s="5">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" t="s" s="5">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s" s="5">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s" s="5">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s" s="5">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" t="s" s="5">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K4" t="s" s="5">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s" s="5">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M4" t="s" s="5">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N4" t="s" s="5">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O4" t="s" s="5">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="R4" t="s" s="5">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="S4" t="s" s="5">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="T4" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="U4" t="s" s="5">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="V4" t="s" s="5">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" t="s" s="5">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s" s="5">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" t="s" s="5">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s" s="5">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s" s="5">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s" s="5">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O5" t="s" s="5">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" t="s" s="5">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="S5" t="s" s="5">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="T5" t="s" s="5">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U5" t="s" s="5">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="V5" t="s" s="5">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" t="s" s="5">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s" s="5">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s" s="5">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s" s="5">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" t="s" s="5">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K6" t="s" s="5">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L6" t="s" s="5">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="M6" t="s" s="5">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="N6" t="s" s="5">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O6" t="s" s="5">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" t="s" s="5">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="R6" t="s" s="5">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="S6" t="s" s="5">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="T6" t="s" s="5">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="U6" t="s" s="5">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="V6" t="s" s="5">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" t="s" s="5">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s" s="5">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s" s="5">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s" s="5">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s" s="5">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" t="s" s="5">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K7" t="s" s="5">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L7" t="s" s="5">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M7" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N7" t="s" s="5">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s" s="5">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" t="s" s="5">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R7" t="s" s="5">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="S7" t="s" s="5">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="T7" t="s" s="5">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="U7" t="s" s="5">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="V7" t="s" s="5">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
@@ -3843,307 +3856,307 @@
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s" s="5">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="G9" t="s" s="5">
+        <v>109</v>
+      </c>
+      <c r="H9" t="s" s="5">
+        <v>110</v>
+      </c>
+      <c r="I9" t="s" s="5">
         <v>104</v>
       </c>
-      <c r="F9" t="s" s="5">
-        <v>105</v>
-      </c>
-      <c r="G9" t="s" s="5">
-        <v>106</v>
-      </c>
-      <c r="H9" t="s" s="5">
-        <v>107</v>
-      </c>
-      <c r="I9" t="s" s="5">
-        <v>101</v>
-      </c>
       <c r="J9" t="s" s="5">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K9" t="s" s="5">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="L9" t="s" s="5">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M9" t="s" s="5">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N9" t="s" s="5">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="O9" t="s" s="5">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="P9" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q9" t="s" s="5">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="R9" t="s" s="5">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="S9" t="s" s="5">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="T9" t="s" s="5">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="U9" t="s" s="5">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="V9" t="s" s="5">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" t="s" s="5">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s" s="5">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s" s="5">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s" s="5">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H10" t="s" s="5">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" t="s" s="5">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K10" t="s" s="5">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L10" t="s" s="5">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="M10" t="s" s="5">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="N10" t="s" s="5">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="O10" t="s" s="5">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" t="s" s="5">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="R10" t="s" s="5">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="S10" t="s" s="5">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="T10" t="s" s="5">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="U10" t="s" s="5">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="V10" t="s" s="5">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" t="s" s="5">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s" s="5">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s" s="5">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F11" t="s" s="5">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H11" t="s" s="5">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" t="s" s="5">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="K11" t="s" s="5">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="L11" t="s" s="5">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="M11" t="s" s="5">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="N11" t="s" s="5">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O11" t="s" s="5">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" t="s" s="5">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="R11" t="s" s="5">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="S11" t="s" s="5">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="T11" t="s" s="5">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="U11" t="s" s="5">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="V11" t="s" s="5">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" t="s" s="5">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s" s="5">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s" s="5">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G12" t="s" s="5">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H12" t="s" s="5">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" t="s" s="5">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="K12" t="s" s="5">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="L12" t="s" s="5">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="M12" t="s" s="5">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N12" t="s" s="5">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="O12" t="s" s="5">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" t="s" s="5">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="R12" t="s" s="5">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="S12" t="s" s="5">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="T12" t="s" s="5">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="U12" t="s" s="5">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="V12" t="s" s="5">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" t="s" s="5">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E13" t="s" s="5">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F13" t="s" s="5">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G13" t="s" s="5">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H13" t="s" s="5">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" t="s" s="5">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K13" t="s" s="5">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="L13" t="s" s="5">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="M13" t="s" s="5">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="N13" t="s" s="5">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="O13" t="s" s="5">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" t="s" s="5">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="R13" t="s" s="5">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="S13" t="s" s="5">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="T13" t="s" s="5">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="U13" t="s" s="5">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="V13" t="s" s="5">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
@@ -4157,307 +4170,307 @@
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s" s="5">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E15" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="F15" t="s" s="5">
+        <v>199</v>
+      </c>
+      <c r="G15" t="s" s="5">
+        <v>200</v>
+      </c>
+      <c r="H15" t="s" s="5">
+        <v>201</v>
+      </c>
+      <c r="I15" t="s" s="5">
         <v>195</v>
       </c>
-      <c r="F15" t="s" s="5">
-        <v>196</v>
-      </c>
-      <c r="G15" t="s" s="5">
-        <v>197</v>
-      </c>
-      <c r="H15" t="s" s="5">
-        <v>198</v>
-      </c>
-      <c r="I15" t="s" s="5">
-        <v>192</v>
-      </c>
       <c r="J15" t="s" s="5">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K15" t="s" s="5">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="L15" t="s" s="5">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="M15" t="s" s="5">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="N15" t="s" s="5">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="O15" t="s" s="5">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="P15" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="Q15" t="s" s="5">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="R15" t="s" s="5">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="S15" t="s" s="5">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="T15" t="s" s="5">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="U15" t="s" s="5">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="V15" t="s" s="5">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" t="s" s="5">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E16" t="s" s="5">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F16" t="s" s="5">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s" s="5">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s" s="5">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" t="s" s="5">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="K16" t="s" s="5">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="L16" t="s" s="5">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="M16" t="s" s="5">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="N16" t="s" s="5">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="O16" t="s" s="5">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" t="s" s="5">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R16" t="s" s="5">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="S16" t="s" s="5">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="T16" t="s" s="5">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="U16" t="s" s="5">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="V16" t="s" s="5">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" t="s" s="5">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s" s="5">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F17" t="s" s="5">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G17" t="s" s="5">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H17" t="s" s="5">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" t="s" s="5">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="K17" t="s" s="5">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="L17" t="s" s="5">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="M17" t="s" s="5">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="N17" t="s" s="5">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="O17" t="s" s="5">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" t="s" s="5">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="R17" t="s" s="5">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="S17" t="s" s="5">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="T17" t="s" s="5">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="U17" t="s" s="5">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="V17" t="s" s="5">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" t="s" s="5">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E18" t="s" s="5">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F18" t="s" s="5">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G18" t="s" s="5">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="H18" t="s" s="5">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" t="s" s="5">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K18" t="s" s="5">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="L18" t="s" s="5">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="M18" t="s" s="5">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="N18" t="s" s="5">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O18" t="s" s="5">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" t="s" s="5">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="R18" t="s" s="5">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="S18" t="s" s="5">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="T18" t="s" s="5">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="U18" t="s" s="5">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="V18" t="s" s="5">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" t="s" s="5">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E19" t="s" s="5">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F19" t="s" s="5">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="G19" t="s" s="5">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="H19" t="s" s="5">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" t="s" s="5">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="K19" t="s" s="5">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="L19" t="s" s="5">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="M19" t="s" s="5">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="N19" t="s" s="5">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="O19" t="s" s="5">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" t="s" s="5">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="R19" t="s" s="5">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="S19" t="s" s="5">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="T19" t="s" s="5">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="U19" t="s" s="5">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="V19" t="s" s="5">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
@@ -4471,316 +4484,316 @@
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" t="s" s="5">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C21" t="s" s="5">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E21" t="s" s="5">
+        <v>289</v>
+      </c>
+      <c r="F21" t="s" s="5">
+        <v>290</v>
+      </c>
+      <c r="G21" t="s" s="5">
+        <v>291</v>
+      </c>
+      <c r="H21" t="s" s="5">
+        <v>292</v>
+      </c>
+      <c r="I21" t="s" s="5">
         <v>286</v>
       </c>
-      <c r="F21" t="s" s="5">
-        <v>287</v>
-      </c>
-      <c r="G21" t="s" s="5">
-        <v>288</v>
-      </c>
-      <c r="H21" t="s" s="5">
-        <v>289</v>
-      </c>
-      <c r="I21" t="s" s="5">
-        <v>283</v>
-      </c>
       <c r="J21" t="s" s="5">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="K21" t="s" s="5">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L21" t="s" s="5">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="M21" t="s" s="5">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="N21" t="s" s="5">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="O21" t="s" s="5">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="P21" t="s" s="5">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="Q21" t="s" s="5">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="R21" t="s" s="5">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="S21" t="s" s="5">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="T21" t="s" s="5">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="U21" t="s" s="5">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="V21" t="s" s="5">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" t="s" s="5">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E22" t="s" s="5">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F22" t="s" s="5">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="G22" t="s" s="5">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="H22" t="s" s="5">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" t="s" s="5">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="K22" t="s" s="5">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="L22" t="s" s="5">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="M22" t="s" s="5">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="N22" t="s" s="5">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O22" t="s" s="5">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" t="s" s="5">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="R22" t="s" s="5">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="S22" t="s" s="5">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="T22" t="s" s="5">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="U22" t="s" s="5">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="V22" t="s" s="5">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" t="s" s="5">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D23" t="s" s="5">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E23" t="s" s="5">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="F23" t="s" s="5">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G23" t="s" s="5">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="H23" t="s" s="5">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" t="s" s="5">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="K23" t="s" s="5">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="L23" t="s" s="5">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="M23" t="s" s="5">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="N23" t="s" s="5">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="O23" t="s" s="5">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" t="s" s="5">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="R23" t="s" s="5">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="S23" t="s" s="5">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="T23" t="s" s="5">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="U23" t="s" s="5">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="V23" t="s" s="5">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" t="s" s="5">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D24" t="s" s="5">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E24" t="s" s="5">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F24" t="s" s="5">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="G24" t="s" s="5">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H24" t="s" s="5">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" t="s" s="5">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="K24" t="s" s="5">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L24" t="s" s="5">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="M24" t="s" s="5">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="N24" t="s" s="5">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="O24" t="s" s="5">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" t="s" s="5">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="R24" t="s" s="5">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="S24" t="s" s="5">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="T24" t="s" s="5">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="U24" t="s" s="5">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="V24" t="s" s="5">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" t="s" s="5">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D25" t="s" s="5">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E25" t="s" s="5">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="F25" t="s" s="5">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G25" t="s" s="5">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="H25" t="s" s="5">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" t="s" s="5">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="K25" t="s" s="5">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="L25" t="s" s="5">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="M25" t="s" s="5">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="N25" t="s" s="5">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="O25" t="s" s="5">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" t="s" s="5">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="R25" t="s" s="5">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="S25" t="s" s="5">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="T25" t="s" s="5">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="U25" t="s" s="5">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="V25" t="s" s="5">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="5">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" t="s" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -4789,7 +4802,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="1"/>
       <c r="J27" t="s" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -4798,7 +4811,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="1"/>
       <c r="Q27" t="s" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
@@ -4810,307 +4823,307 @@
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D28" t="s" s="5">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="E28" t="s" s="5">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="F28" t="s" s="5">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G28" t="s" s="5">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="H28" t="s" s="5">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I28" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J28" t="s" s="5">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="K28" t="s" s="5">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="L28" t="s" s="5">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="M28" t="s" s="5">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="N28" t="s" s="5">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="O28" t="s" s="5">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="P28" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q28" t="s" s="5">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="R28" t="s" s="5">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="S28" t="s" s="5">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="T28" t="s" s="5">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="U28" t="s" s="5">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="V28" t="s" s="5">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" t="s" s="5">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D29" t="s" s="5">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E29" t="s" s="5">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="F29" t="s" s="5">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="G29" t="s" s="5">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="H29" t="s" s="5">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" t="s" s="5">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="K29" t="s" s="5">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="L29" t="s" s="5">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="M29" t="s" s="5">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="N29" t="s" s="5">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="O29" t="s" s="5">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" t="s" s="5">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="R29" t="s" s="5">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="S29" t="s" s="5">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="T29" t="s" s="5">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="U29" t="s" s="5">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="V29" t="s" s="5">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" t="s" s="5">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D30" t="s" s="5">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E30" t="s" s="5">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="F30" t="s" s="5">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="G30" t="s" s="5">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="H30" t="s" s="5">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" t="s" s="5">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="K30" t="s" s="5">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="L30" t="s" s="5">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="M30" t="s" s="5">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="N30" t="s" s="5">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="O30" t="s" s="5">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" t="s" s="5">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="R30" t="s" s="5">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="S30" t="s" s="5">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="T30" t="s" s="5">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="U30" t="s" s="5">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="V30" t="s" s="5">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" t="s" s="5">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="D31" t="s" s="5">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="E31" t="s" s="5">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="F31" t="s" s="5">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G31" t="s" s="5">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="H31" t="s" s="5">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" t="s" s="5">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="K31" t="s" s="5">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="L31" t="s" s="5">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="M31" t="s" s="5">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="N31" t="s" s="5">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="O31" t="s" s="5">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" t="s" s="5">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="R31" t="s" s="5">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="S31" t="s" s="5">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="T31" t="s" s="5">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="U31" t="s" s="5">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="V31" t="s" s="5">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" t="s" s="5">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="D32" t="s" s="5">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="E32" t="s" s="5">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="F32" t="s" s="5">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="G32" t="s" s="5">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="H32" t="s" s="5">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" t="s" s="5">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="K32" t="s" s="5">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="L32" t="s" s="5">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="M32" t="s" s="5">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="N32" t="s" s="5">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="O32" t="s" s="5">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" t="s" s="5">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="R32" t="s" s="5">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="S32" t="s" s="5">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="T32" t="s" s="5">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="U32" t="s" s="5">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="V32" t="s" s="5">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
@@ -5119,307 +5132,307 @@
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s" s="5">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D34" t="s" s="5">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="E34" t="s" s="5">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="F34" t="s" s="5">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G34" t="s" s="5">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="H34" t="s" s="5">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="I34" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J34" t="s" s="5">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="K34" t="s" s="5">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="L34" t="s" s="5">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="M34" t="s" s="5">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="N34" t="s" s="5">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="O34" t="s" s="5">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="P34" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q34" t="s" s="5">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="R34" t="s" s="5">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="S34" t="s" s="5">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="T34" t="s" s="5">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="U34" t="s" s="5">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="V34" t="s" s="5">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" t="s" s="5">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="D35" t="s" s="5">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="E35" t="s" s="5">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="F35" t="s" s="5">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="G35" t="s" s="5">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="H35" t="s" s="5">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" t="s" s="5">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="K35" t="s" s="5">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="L35" t="s" s="5">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="M35" t="s" s="5">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="N35" t="s" s="5">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="O35" t="s" s="5">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" t="s" s="5">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="R35" t="s" s="5">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="S35" t="s" s="5">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="T35" t="s" s="5">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="U35" t="s" s="5">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="V35" t="s" s="5">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" t="s" s="5">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D36" t="s" s="5">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E36" t="s" s="5">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="F36" t="s" s="5">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="G36" t="s" s="5">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="H36" t="s" s="5">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" t="s" s="5">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="K36" t="s" s="5">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="L36" t="s" s="5">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="M36" t="s" s="5">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="N36" t="s" s="5">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="O36" t="s" s="5">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="P36" s="5"/>
       <c r="Q36" t="s" s="5">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="R36" t="s" s="5">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="S36" t="s" s="5">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="T36" t="s" s="5">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="U36" t="s" s="5">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="V36" t="s" s="5">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" t="s" s="5">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="E37" t="s" s="5">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="F37" t="s" s="5">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="G37" t="s" s="5">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="H37" t="s" s="5">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" t="s" s="5">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="K37" t="s" s="5">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="L37" t="s" s="5">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="M37" t="s" s="5">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="N37" t="s" s="5">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="O37" t="s" s="5">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" t="s" s="5">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="R37" t="s" s="5">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="S37" t="s" s="5">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="T37" t="s" s="5">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="U37" t="s" s="5">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="V37" t="s" s="5">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" t="s" s="5">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E38" t="s" s="5">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="F38" t="s" s="5">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="G38" t="s" s="5">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="H38" t="s" s="5">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" t="s" s="5">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="K38" t="s" s="5">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="L38" t="s" s="5">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="M38" t="s" s="5">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="N38" t="s" s="5">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="O38" t="s" s="5">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="P38" s="5"/>
       <c r="Q38" t="s" s="5">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="R38" t="s" s="5">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="S38" t="s" s="5">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="T38" t="s" s="5">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="U38" t="s" s="5">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="V38" t="s" s="5">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
@@ -5428,307 +5441,307 @@
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="D40" t="s" s="5">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E40" t="s" s="5">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="F40" t="s" s="5">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="G40" t="s" s="5">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="H40" t="s" s="5">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="I40" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J40" t="s" s="5">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="K40" t="s" s="5">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="L40" t="s" s="5">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="M40" t="s" s="5">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="N40" t="s" s="5">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="O40" t="s" s="5">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="P40" t="s" s="5">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="Q40" t="s" s="5">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="R40" t="s" s="5">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="S40" t="s" s="5">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="T40" t="s" s="5">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="U40" t="s" s="5">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="V40" t="s" s="5">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" t="s" s="5">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D41" t="s" s="5">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E41" t="s" s="5">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="F41" t="s" s="5">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="G41" t="s" s="5">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="H41" t="s" s="5">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" t="s" s="5">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="K41" t="s" s="5">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="L41" t="s" s="5">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="M41" t="s" s="5">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="N41" t="s" s="5">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="O41" t="s" s="5">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="P41" s="5"/>
       <c r="Q41" t="s" s="5">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="R41" t="s" s="5">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="S41" t="s" s="5">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="T41" t="s" s="5">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="U41" t="s" s="5">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="V41" t="s" s="5">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" t="s" s="5">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="D42" t="s" s="5">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="E42" t="s" s="5">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="F42" t="s" s="5">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="G42" t="s" s="5">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="H42" t="s" s="5">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" t="s" s="5">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="K42" t="s" s="5">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="L42" t="s" s="5">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="M42" t="s" s="5">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="N42" t="s" s="5">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="O42" t="s" s="5">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" t="s" s="5">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="R42" t="s" s="5">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="S42" t="s" s="5">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="T42" t="s" s="5">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="U42" t="s" s="5">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="V42" t="s" s="5">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" t="s" s="5">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="D43" t="s" s="5">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="E43" t="s" s="5">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="F43" t="s" s="5">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="G43" t="s" s="5">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="H43" t="s" s="5">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" t="s" s="5">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="K43" t="s" s="5">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="L43" t="s" s="5">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="M43" t="s" s="5">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="N43" t="s" s="5">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="O43" t="s" s="5">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" t="s" s="5">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="R43" t="s" s="5">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="S43" t="s" s="5">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="T43" t="s" s="5">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="U43" t="s" s="5">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="V43" t="s" s="5">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" t="s" s="5">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D44" t="s" s="5">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="E44" t="s" s="5">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="F44" t="s" s="5">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="G44" t="s" s="5">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="H44" t="s" s="5">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" t="s" s="5">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="K44" t="s" s="5">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="L44" t="s" s="5">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="M44" t="s" s="5">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="N44" t="s" s="5">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="O44" t="s" s="5">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" t="s" s="5">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="R44" t="s" s="5">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="S44" t="s" s="5">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="T44" t="s" s="5">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="U44" t="s" s="5">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="V44" t="s" s="5">
-        <v>644</v>
+        <v>647</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
@@ -5737,307 +5750,307 @@
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" t="s" s="5">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D46" t="s" s="5">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="E46" t="s" s="5">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F46" t="s" s="5">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="G46" t="s" s="5">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="H46" t="s" s="5">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="I46" t="s" s="5">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="J46" t="s" s="5">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="K46" t="s" s="5">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="L46" t="s" s="5">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="M46" t="s" s="5">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="N46" t="s" s="5">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="O46" t="s" s="5">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="P46" t="s" s="5">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="Q46" t="s" s="5">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="R46" t="s" s="5">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="S46" t="s" s="5">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="T46" t="s" s="5">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="U46" t="s" s="5">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="V46" t="s" s="5">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" t="s" s="5">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="D47" t="s" s="5">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="E47" t="s" s="5">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="F47" t="s" s="5">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G47" t="s" s="5">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="H47" t="s" s="5">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" t="s" s="5">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="K47" t="s" s="5">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="L47" t="s" s="5">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M47" t="s" s="5">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="N47" t="s" s="5">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="O47" t="s" s="5">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="P47" s="5"/>
       <c r="Q47" t="s" s="5">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="R47" t="s" s="5">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="S47" t="s" s="5">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="T47" t="s" s="5">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="U47" t="s" s="5">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="V47" t="s" s="5">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" t="s" s="5">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="D48" t="s" s="5">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E48" t="s" s="5">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="F48" t="s" s="5">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="G48" t="s" s="5">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="H48" t="s" s="5">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" t="s" s="5">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="K48" t="s" s="5">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="L48" t="s" s="5">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="M48" t="s" s="5">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="N48" t="s" s="5">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="O48" t="s" s="5">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" t="s" s="5">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="R48" t="s" s="5">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="S48" t="s" s="5">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="T48" t="s" s="5">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="U48" t="s" s="5">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="V48" t="s" s="5">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" t="s" s="5">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="D49" t="s" s="5">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="E49" t="s" s="5">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="F49" t="s" s="5">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="G49" t="s" s="5">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="H49" t="s" s="5">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" t="s" s="5">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="K49" t="s" s="5">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="L49" t="s" s="5">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="M49" t="s" s="5">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="N49" t="s" s="5">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="O49" t="s" s="5">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" t="s" s="5">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="R49" t="s" s="5">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="S49" t="s" s="5">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="T49" t="s" s="5">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="U49" t="s" s="5">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="V49" t="s" s="5">
-        <v>716</v>
+        <v>719</v>
       </c>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" t="s" s="5">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="D50" t="s" s="5">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="E50" t="s" s="5">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="F50" t="s" s="5">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="G50" t="s" s="5">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="H50" t="s" s="5">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" t="s" s="5">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="K50" t="s" s="5">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="L50" t="s" s="5">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="M50" t="s" s="5">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="N50" t="s" s="5">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="O50" t="s" s="5">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="P50" s="5"/>
       <c r="Q50" t="s" s="5">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="R50" t="s" s="5">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="S50" t="s" s="5">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="T50" t="s" s="5">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="U50" t="s" s="5">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="V50" t="s" s="5">
-        <v>734</v>
+        <v>737</v>
       </c>
     </row>
     <row r="52">
@@ -6087,4 +6100,1322 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="9" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="9" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.3516" style="9" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.3516" style="9" customWidth="1"/>
+    <col min="14" max="14" width="16.3516" style="9" customWidth="1"/>
+    <col min="15" max="15" width="16.3516" style="9" customWidth="1"/>
+    <col min="16" max="16" width="16.3516" style="9" customWidth="1"/>
+    <col min="17" max="17" width="16.3516" style="9" customWidth="1"/>
+    <col min="18" max="18" width="16.3516" style="9" customWidth="1"/>
+    <col min="19" max="19" width="16.3516" style="9" customWidth="1"/>
+    <col min="20" max="20" width="16.3516" style="9" customWidth="1"/>
+    <col min="21" max="21" width="16.3516" style="9" customWidth="1"/>
+    <col min="22" max="22" width="16.3516" style="9" customWidth="1"/>
+    <col min="23" max="23" width="16.3516" style="9" customWidth="1"/>
+    <col min="24" max="24" width="16.3516" style="9" customWidth="1"/>
+    <col min="25" max="25" width="16.3516" style="9" customWidth="1"/>
+    <col min="26" max="26" width="16.3516" style="9" customWidth="1"/>
+    <col min="27" max="27" width="16.3516" style="9" customWidth="1"/>
+    <col min="28" max="28" width="16.3516" style="9" customWidth="1"/>
+    <col min="29" max="16384" width="16.3516" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="I2" t="s" s="5">
+        <v>104</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="P2" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="W2" t="s" s="5">
+        <v>286</v>
+      </c>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AD2" s="9"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="5">
+        <v>378</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>379</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>380</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>381</v>
+      </c>
+      <c r="F3" t="s" s="5">
+        <v>382</v>
+      </c>
+      <c r="G3" t="s" s="5">
+        <v>383</v>
+      </c>
+      <c r="I3" t="s" s="5">
+        <v>468</v>
+      </c>
+      <c r="J3" t="s" s="5">
+        <v>469</v>
+      </c>
+      <c r="K3" t="s" s="5">
+        <v>470</v>
+      </c>
+      <c r="L3" t="s" s="5">
+        <v>471</v>
+      </c>
+      <c r="M3" t="s" s="5">
+        <v>472</v>
+      </c>
+      <c r="N3" t="s" s="5">
+        <v>473</v>
+      </c>
+      <c r="P3" t="s" s="5">
+        <v>558</v>
+      </c>
+      <c r="Q3" t="s" s="5">
+        <v>559</v>
+      </c>
+      <c r="R3" t="s" s="5">
+        <v>560</v>
+      </c>
+      <c r="S3" t="s" s="5">
+        <v>561</v>
+      </c>
+      <c r="T3" t="s" s="5">
+        <v>562</v>
+      </c>
+      <c r="U3" t="s" s="5">
+        <v>563</v>
+      </c>
+      <c r="W3" t="s" s="5">
+        <v>648</v>
+      </c>
+      <c r="X3" t="s" s="5">
+        <v>649</v>
+      </c>
+      <c r="Y3" t="s" s="5">
+        <v>650</v>
+      </c>
+      <c r="Z3" t="s" s="5">
+        <v>651</v>
+      </c>
+      <c r="AA3" t="s" s="5">
+        <v>652</v>
+      </c>
+      <c r="AB3" t="s" s="5">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s" s="5">
+        <v>396</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>397</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>398</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>399</v>
+      </c>
+      <c r="F4" t="s" s="5">
+        <v>400</v>
+      </c>
+      <c r="G4" t="s" s="5">
+        <v>401</v>
+      </c>
+      <c r="I4" t="s" s="5">
+        <v>486</v>
+      </c>
+      <c r="J4" t="s" s="5">
+        <v>487</v>
+      </c>
+      <c r="K4" t="s" s="5">
+        <v>488</v>
+      </c>
+      <c r="L4" t="s" s="5">
+        <v>489</v>
+      </c>
+      <c r="M4" t="s" s="5">
+        <v>490</v>
+      </c>
+      <c r="N4" t="s" s="5">
+        <v>491</v>
+      </c>
+      <c r="P4" t="s" s="5">
+        <v>576</v>
+      </c>
+      <c r="Q4" t="s" s="5">
+        <v>577</v>
+      </c>
+      <c r="R4" t="s" s="5">
+        <v>578</v>
+      </c>
+      <c r="S4" t="s" s="5">
+        <v>579</v>
+      </c>
+      <c r="T4" t="s" s="5">
+        <v>580</v>
+      </c>
+      <c r="U4" t="s" s="5">
+        <v>581</v>
+      </c>
+      <c r="W4" t="s" s="5">
+        <v>666</v>
+      </c>
+      <c r="X4" t="s" s="5">
+        <v>667</v>
+      </c>
+      <c r="Y4" t="s" s="5">
+        <v>668</v>
+      </c>
+      <c r="Z4" t="s" s="5">
+        <v>669</v>
+      </c>
+      <c r="AA4" t="s" s="5">
+        <v>670</v>
+      </c>
+      <c r="AB4" t="s" s="5">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s" s="5">
+        <v>414</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>415</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>416</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>417</v>
+      </c>
+      <c r="F5" t="s" s="5">
+        <v>418</v>
+      </c>
+      <c r="G5" t="s" s="5">
+        <v>419</v>
+      </c>
+      <c r="I5" t="s" s="5">
+        <v>504</v>
+      </c>
+      <c r="J5" t="s" s="5">
+        <v>505</v>
+      </c>
+      <c r="K5" t="s" s="5">
+        <v>506</v>
+      </c>
+      <c r="L5" t="s" s="5">
+        <v>507</v>
+      </c>
+      <c r="M5" t="s" s="5">
+        <v>508</v>
+      </c>
+      <c r="N5" t="s" s="5">
+        <v>509</v>
+      </c>
+      <c r="P5" t="s" s="5">
+        <v>594</v>
+      </c>
+      <c r="Q5" t="s" s="5">
+        <v>595</v>
+      </c>
+      <c r="R5" t="s" s="5">
+        <v>596</v>
+      </c>
+      <c r="S5" t="s" s="5">
+        <v>597</v>
+      </c>
+      <c r="T5" t="s" s="5">
+        <v>598</v>
+      </c>
+      <c r="U5" t="s" s="5">
+        <v>599</v>
+      </c>
+      <c r="W5" t="s" s="5">
+        <v>684</v>
+      </c>
+      <c r="X5" t="s" s="5">
+        <v>685</v>
+      </c>
+      <c r="Y5" t="s" s="5">
+        <v>686</v>
+      </c>
+      <c r="Z5" t="s" s="5">
+        <v>687</v>
+      </c>
+      <c r="AA5" t="s" s="5">
+        <v>688</v>
+      </c>
+      <c r="AB5" t="s" s="5">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s" s="5">
+        <v>432</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>433</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>434</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>435</v>
+      </c>
+      <c r="F6" t="s" s="5">
+        <v>436</v>
+      </c>
+      <c r="G6" t="s" s="5">
+        <v>437</v>
+      </c>
+      <c r="I6" t="s" s="5">
+        <v>522</v>
+      </c>
+      <c r="J6" t="s" s="5">
+        <v>523</v>
+      </c>
+      <c r="K6" t="s" s="5">
+        <v>524</v>
+      </c>
+      <c r="L6" t="s" s="5">
+        <v>525</v>
+      </c>
+      <c r="M6" t="s" s="5">
+        <v>526</v>
+      </c>
+      <c r="N6" t="s" s="5">
+        <v>527</v>
+      </c>
+      <c r="P6" t="s" s="5">
+        <v>612</v>
+      </c>
+      <c r="Q6" t="s" s="5">
+        <v>613</v>
+      </c>
+      <c r="R6" t="s" s="5">
+        <v>614</v>
+      </c>
+      <c r="S6" t="s" s="5">
+        <v>615</v>
+      </c>
+      <c r="T6" t="s" s="5">
+        <v>616</v>
+      </c>
+      <c r="U6" t="s" s="5">
+        <v>617</v>
+      </c>
+      <c r="W6" t="s" s="5">
+        <v>702</v>
+      </c>
+      <c r="X6" t="s" s="5">
+        <v>703</v>
+      </c>
+      <c r="Y6" t="s" s="5">
+        <v>704</v>
+      </c>
+      <c r="Z6" t="s" s="5">
+        <v>705</v>
+      </c>
+      <c r="AA6" t="s" s="5">
+        <v>706</v>
+      </c>
+      <c r="AB6" t="s" s="5">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s" s="5">
+        <v>450</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>451</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>452</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>453</v>
+      </c>
+      <c r="F7" t="s" s="5">
+        <v>454</v>
+      </c>
+      <c r="G7" t="s" s="5">
+        <v>455</v>
+      </c>
+      <c r="I7" t="s" s="5">
+        <v>540</v>
+      </c>
+      <c r="J7" t="s" s="5">
+        <v>541</v>
+      </c>
+      <c r="K7" t="s" s="5">
+        <v>542</v>
+      </c>
+      <c r="L7" t="s" s="5">
+        <v>543</v>
+      </c>
+      <c r="M7" t="s" s="5">
+        <v>544</v>
+      </c>
+      <c r="N7" t="s" s="5">
+        <v>545</v>
+      </c>
+      <c r="P7" t="s" s="5">
+        <v>630</v>
+      </c>
+      <c r="Q7" t="s" s="5">
+        <v>631</v>
+      </c>
+      <c r="R7" t="s" s="5">
+        <v>632</v>
+      </c>
+      <c r="S7" t="s" s="5">
+        <v>633</v>
+      </c>
+      <c r="T7" t="s" s="5">
+        <v>634</v>
+      </c>
+      <c r="U7" t="s" s="5">
+        <v>635</v>
+      </c>
+      <c r="W7" t="s" s="5">
+        <v>720</v>
+      </c>
+      <c r="X7" t="s" s="5">
+        <v>721</v>
+      </c>
+      <c r="Y7" t="s" s="5">
+        <v>722</v>
+      </c>
+      <c r="Z7" t="s" s="5">
+        <v>723</v>
+      </c>
+      <c r="AA7" t="s" s="5">
+        <v>724</v>
+      </c>
+      <c r="AB7" t="s" s="5">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="I8" t="s" s="5">
+        <v>104</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="P8" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="W8" t="s" s="5">
+        <v>286</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AD8" s="9"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="5">
+        <v>384</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>385</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>386</v>
+      </c>
+      <c r="E9" t="s" s="5">
+        <v>387</v>
+      </c>
+      <c r="F9" t="s" s="5">
+        <v>388</v>
+      </c>
+      <c r="G9" t="s" s="5">
+        <v>389</v>
+      </c>
+      <c r="I9" t="s" s="5">
+        <v>474</v>
+      </c>
+      <c r="J9" t="s" s="5">
+        <v>475</v>
+      </c>
+      <c r="K9" t="s" s="5">
+        <v>476</v>
+      </c>
+      <c r="L9" t="s" s="5">
+        <v>477</v>
+      </c>
+      <c r="M9" t="s" s="5">
+        <v>478</v>
+      </c>
+      <c r="N9" t="s" s="5">
+        <v>479</v>
+      </c>
+      <c r="P9" t="s" s="5">
+        <v>564</v>
+      </c>
+      <c r="Q9" t="s" s="5">
+        <v>565</v>
+      </c>
+      <c r="R9" t="s" s="5">
+        <v>566</v>
+      </c>
+      <c r="S9" t="s" s="5">
+        <v>567</v>
+      </c>
+      <c r="T9" t="s" s="5">
+        <v>568</v>
+      </c>
+      <c r="U9" t="s" s="5">
+        <v>569</v>
+      </c>
+      <c r="W9" t="s" s="5">
+        <v>654</v>
+      </c>
+      <c r="X9" t="s" s="5">
+        <v>655</v>
+      </c>
+      <c r="Y9" t="s" s="5">
+        <v>656</v>
+      </c>
+      <c r="Z9" t="s" s="5">
+        <v>657</v>
+      </c>
+      <c r="AA9" t="s" s="5">
+        <v>658</v>
+      </c>
+      <c r="AB9" t="s" s="5">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s" s="5">
+        <v>402</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>403</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>404</v>
+      </c>
+      <c r="E10" t="s" s="5">
+        <v>405</v>
+      </c>
+      <c r="F10" t="s" s="5">
+        <v>406</v>
+      </c>
+      <c r="G10" t="s" s="5">
+        <v>407</v>
+      </c>
+      <c r="I10" t="s" s="5">
+        <v>492</v>
+      </c>
+      <c r="J10" t="s" s="5">
+        <v>493</v>
+      </c>
+      <c r="K10" t="s" s="5">
+        <v>494</v>
+      </c>
+      <c r="L10" t="s" s="5">
+        <v>495</v>
+      </c>
+      <c r="M10" t="s" s="5">
+        <v>496</v>
+      </c>
+      <c r="N10" t="s" s="5">
+        <v>497</v>
+      </c>
+      <c r="P10" t="s" s="5">
+        <v>582</v>
+      </c>
+      <c r="Q10" t="s" s="5">
+        <v>583</v>
+      </c>
+      <c r="R10" t="s" s="5">
+        <v>584</v>
+      </c>
+      <c r="S10" t="s" s="5">
+        <v>585</v>
+      </c>
+      <c r="T10" t="s" s="5">
+        <v>586</v>
+      </c>
+      <c r="U10" t="s" s="5">
+        <v>587</v>
+      </c>
+      <c r="W10" t="s" s="5">
+        <v>672</v>
+      </c>
+      <c r="X10" t="s" s="5">
+        <v>673</v>
+      </c>
+      <c r="Y10" t="s" s="5">
+        <v>674</v>
+      </c>
+      <c r="Z10" t="s" s="5">
+        <v>675</v>
+      </c>
+      <c r="AA10" t="s" s="5">
+        <v>676</v>
+      </c>
+      <c r="AB10" t="s" s="5">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="5">
+        <v>420</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>421</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>422</v>
+      </c>
+      <c r="E11" t="s" s="5">
+        <v>423</v>
+      </c>
+      <c r="F11" t="s" s="5">
+        <v>424</v>
+      </c>
+      <c r="G11" t="s" s="5">
+        <v>425</v>
+      </c>
+      <c r="I11" t="s" s="5">
+        <v>510</v>
+      </c>
+      <c r="J11" t="s" s="5">
+        <v>511</v>
+      </c>
+      <c r="K11" t="s" s="5">
+        <v>512</v>
+      </c>
+      <c r="L11" t="s" s="5">
+        <v>513</v>
+      </c>
+      <c r="M11" t="s" s="5">
+        <v>514</v>
+      </c>
+      <c r="N11" t="s" s="5">
+        <v>515</v>
+      </c>
+      <c r="P11" t="s" s="5">
+        <v>600</v>
+      </c>
+      <c r="Q11" t="s" s="5">
+        <v>601</v>
+      </c>
+      <c r="R11" t="s" s="5">
+        <v>602</v>
+      </c>
+      <c r="S11" t="s" s="5">
+        <v>603</v>
+      </c>
+      <c r="T11" t="s" s="5">
+        <v>604</v>
+      </c>
+      <c r="U11" t="s" s="5">
+        <v>605</v>
+      </c>
+      <c r="W11" t="s" s="5">
+        <v>690</v>
+      </c>
+      <c r="X11" t="s" s="5">
+        <v>691</v>
+      </c>
+      <c r="Y11" t="s" s="5">
+        <v>692</v>
+      </c>
+      <c r="Z11" t="s" s="5">
+        <v>693</v>
+      </c>
+      <c r="AA11" t="s" s="5">
+        <v>694</v>
+      </c>
+      <c r="AB11" t="s" s="5">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s" s="5">
+        <v>438</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>439</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>440</v>
+      </c>
+      <c r="E12" t="s" s="5">
+        <v>441</v>
+      </c>
+      <c r="F12" t="s" s="5">
+        <v>442</v>
+      </c>
+      <c r="G12" t="s" s="5">
+        <v>443</v>
+      </c>
+      <c r="I12" t="s" s="5">
+        <v>528</v>
+      </c>
+      <c r="J12" t="s" s="5">
+        <v>529</v>
+      </c>
+      <c r="K12" t="s" s="5">
+        <v>530</v>
+      </c>
+      <c r="L12" t="s" s="5">
+        <v>531</v>
+      </c>
+      <c r="M12" t="s" s="5">
+        <v>532</v>
+      </c>
+      <c r="N12" t="s" s="5">
+        <v>533</v>
+      </c>
+      <c r="P12" t="s" s="5">
+        <v>618</v>
+      </c>
+      <c r="Q12" t="s" s="5">
+        <v>619</v>
+      </c>
+      <c r="R12" t="s" s="5">
+        <v>620</v>
+      </c>
+      <c r="S12" t="s" s="5">
+        <v>621</v>
+      </c>
+      <c r="T12" t="s" s="5">
+        <v>622</v>
+      </c>
+      <c r="U12" t="s" s="5">
+        <v>623</v>
+      </c>
+      <c r="W12" t="s" s="5">
+        <v>708</v>
+      </c>
+      <c r="X12" t="s" s="5">
+        <v>709</v>
+      </c>
+      <c r="Y12" t="s" s="5">
+        <v>710</v>
+      </c>
+      <c r="Z12" t="s" s="5">
+        <v>711</v>
+      </c>
+      <c r="AA12" t="s" s="5">
+        <v>712</v>
+      </c>
+      <c r="AB12" t="s" s="5">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="6"/>
+      <c r="B13" t="s" s="5">
+        <v>456</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>457</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>458</v>
+      </c>
+      <c r="E13" t="s" s="5">
+        <v>459</v>
+      </c>
+      <c r="F13" t="s" s="5">
+        <v>460</v>
+      </c>
+      <c r="G13" t="s" s="5">
+        <v>461</v>
+      </c>
+      <c r="I13" t="s" s="5">
+        <v>546</v>
+      </c>
+      <c r="J13" t="s" s="5">
+        <v>547</v>
+      </c>
+      <c r="K13" t="s" s="5">
+        <v>548</v>
+      </c>
+      <c r="L13" t="s" s="5">
+        <v>549</v>
+      </c>
+      <c r="M13" t="s" s="5">
+        <v>550</v>
+      </c>
+      <c r="N13" t="s" s="5">
+        <v>551</v>
+      </c>
+      <c r="P13" t="s" s="5">
+        <v>636</v>
+      </c>
+      <c r="Q13" t="s" s="5">
+        <v>637</v>
+      </c>
+      <c r="R13" t="s" s="5">
+        <v>638</v>
+      </c>
+      <c r="S13" t="s" s="5">
+        <v>639</v>
+      </c>
+      <c r="T13" t="s" s="5">
+        <v>640</v>
+      </c>
+      <c r="U13" t="s" s="5">
+        <v>641</v>
+      </c>
+      <c r="W13" t="s" s="5">
+        <v>726</v>
+      </c>
+      <c r="X13" t="s" s="5">
+        <v>727</v>
+      </c>
+      <c r="Y13" t="s" s="5">
+        <v>728</v>
+      </c>
+      <c r="Z13" t="s" s="5">
+        <v>729</v>
+      </c>
+      <c r="AA13" t="s" s="5">
+        <v>730</v>
+      </c>
+      <c r="AB13" t="s" s="5">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="I14" t="s" s="5">
+        <v>104</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="P14" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="W14" t="s" s="5">
+        <v>286</v>
+      </c>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AD14" s="9"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s" s="5">
+        <v>390</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>391</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>392</v>
+      </c>
+      <c r="E15" t="s" s="5">
+        <v>393</v>
+      </c>
+      <c r="F15" t="s" s="5">
+        <v>394</v>
+      </c>
+      <c r="G15" t="s" s="5">
+        <v>395</v>
+      </c>
+      <c r="I15" t="s" s="5">
+        <v>480</v>
+      </c>
+      <c r="J15" t="s" s="5">
+        <v>481</v>
+      </c>
+      <c r="K15" t="s" s="5">
+        <v>482</v>
+      </c>
+      <c r="L15" t="s" s="5">
+        <v>483</v>
+      </c>
+      <c r="M15" t="s" s="5">
+        <v>484</v>
+      </c>
+      <c r="N15" t="s" s="5">
+        <v>485</v>
+      </c>
+      <c r="P15" t="s" s="5">
+        <v>570</v>
+      </c>
+      <c r="Q15" t="s" s="5">
+        <v>571</v>
+      </c>
+      <c r="R15" t="s" s="5">
+        <v>572</v>
+      </c>
+      <c r="S15" t="s" s="5">
+        <v>573</v>
+      </c>
+      <c r="T15" t="s" s="5">
+        <v>574</v>
+      </c>
+      <c r="U15" t="s" s="5">
+        <v>575</v>
+      </c>
+      <c r="W15" t="s" s="5">
+        <v>660</v>
+      </c>
+      <c r="X15" t="s" s="5">
+        <v>661</v>
+      </c>
+      <c r="Y15" t="s" s="5">
+        <v>662</v>
+      </c>
+      <c r="Z15" t="s" s="5">
+        <v>663</v>
+      </c>
+      <c r="AA15" t="s" s="5">
+        <v>664</v>
+      </c>
+      <c r="AB15" t="s" s="5">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s" s="5">
+        <v>408</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>409</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>410</v>
+      </c>
+      <c r="E16" t="s" s="5">
+        <v>411</v>
+      </c>
+      <c r="F16" t="s" s="5">
+        <v>412</v>
+      </c>
+      <c r="G16" t="s" s="5">
+        <v>413</v>
+      </c>
+      <c r="I16" t="s" s="5">
+        <v>498</v>
+      </c>
+      <c r="J16" t="s" s="5">
+        <v>499</v>
+      </c>
+      <c r="K16" t="s" s="5">
+        <v>500</v>
+      </c>
+      <c r="L16" t="s" s="5">
+        <v>501</v>
+      </c>
+      <c r="M16" t="s" s="5">
+        <v>502</v>
+      </c>
+      <c r="N16" t="s" s="5">
+        <v>503</v>
+      </c>
+      <c r="P16" t="s" s="5">
+        <v>588</v>
+      </c>
+      <c r="Q16" t="s" s="5">
+        <v>589</v>
+      </c>
+      <c r="R16" t="s" s="5">
+        <v>590</v>
+      </c>
+      <c r="S16" t="s" s="5">
+        <v>591</v>
+      </c>
+      <c r="T16" t="s" s="5">
+        <v>592</v>
+      </c>
+      <c r="U16" t="s" s="5">
+        <v>593</v>
+      </c>
+      <c r="W16" t="s" s="5">
+        <v>678</v>
+      </c>
+      <c r="X16" t="s" s="5">
+        <v>679</v>
+      </c>
+      <c r="Y16" t="s" s="5">
+        <v>680</v>
+      </c>
+      <c r="Z16" t="s" s="5">
+        <v>681</v>
+      </c>
+      <c r="AA16" t="s" s="5">
+        <v>682</v>
+      </c>
+      <c r="AB16" t="s" s="5">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" t="s" s="5">
+        <v>426</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>427</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>428</v>
+      </c>
+      <c r="E17" t="s" s="5">
+        <v>429</v>
+      </c>
+      <c r="F17" t="s" s="5">
+        <v>430</v>
+      </c>
+      <c r="G17" t="s" s="5">
+        <v>431</v>
+      </c>
+      <c r="I17" t="s" s="5">
+        <v>516</v>
+      </c>
+      <c r="J17" t="s" s="5">
+        <v>517</v>
+      </c>
+      <c r="K17" t="s" s="5">
+        <v>518</v>
+      </c>
+      <c r="L17" t="s" s="5">
+        <v>519</v>
+      </c>
+      <c r="M17" t="s" s="5">
+        <v>520</v>
+      </c>
+      <c r="N17" t="s" s="5">
+        <v>521</v>
+      </c>
+      <c r="P17" t="s" s="5">
+        <v>606</v>
+      </c>
+      <c r="Q17" t="s" s="5">
+        <v>607</v>
+      </c>
+      <c r="R17" t="s" s="5">
+        <v>608</v>
+      </c>
+      <c r="S17" t="s" s="5">
+        <v>609</v>
+      </c>
+      <c r="T17" t="s" s="5">
+        <v>610</v>
+      </c>
+      <c r="U17" t="s" s="5">
+        <v>611</v>
+      </c>
+      <c r="W17" t="s" s="5">
+        <v>696</v>
+      </c>
+      <c r="X17" t="s" s="5">
+        <v>697</v>
+      </c>
+      <c r="Y17" t="s" s="5">
+        <v>698</v>
+      </c>
+      <c r="Z17" t="s" s="5">
+        <v>699</v>
+      </c>
+      <c r="AA17" t="s" s="5">
+        <v>700</v>
+      </c>
+      <c r="AB17" t="s" s="5">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s" s="5">
+        <v>444</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>445</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>446</v>
+      </c>
+      <c r="E18" t="s" s="5">
+        <v>447</v>
+      </c>
+      <c r="F18" t="s" s="5">
+        <v>448</v>
+      </c>
+      <c r="G18" t="s" s="5">
+        <v>449</v>
+      </c>
+      <c r="I18" t="s" s="5">
+        <v>534</v>
+      </c>
+      <c r="J18" t="s" s="5">
+        <v>535</v>
+      </c>
+      <c r="K18" t="s" s="5">
+        <v>536</v>
+      </c>
+      <c r="L18" t="s" s="5">
+        <v>537</v>
+      </c>
+      <c r="M18" t="s" s="5">
+        <v>538</v>
+      </c>
+      <c r="N18" t="s" s="5">
+        <v>539</v>
+      </c>
+      <c r="P18" t="s" s="5">
+        <v>624</v>
+      </c>
+      <c r="Q18" t="s" s="5">
+        <v>625</v>
+      </c>
+      <c r="R18" t="s" s="5">
+        <v>626</v>
+      </c>
+      <c r="S18" t="s" s="5">
+        <v>627</v>
+      </c>
+      <c r="T18" t="s" s="5">
+        <v>628</v>
+      </c>
+      <c r="U18" t="s" s="5">
+        <v>629</v>
+      </c>
+      <c r="W18" t="s" s="5">
+        <v>714</v>
+      </c>
+      <c r="X18" t="s" s="5">
+        <v>715</v>
+      </c>
+      <c r="Y18" t="s" s="5">
+        <v>716</v>
+      </c>
+      <c r="Z18" t="s" s="5">
+        <v>717</v>
+      </c>
+      <c r="AA18" t="s" s="5">
+        <v>718</v>
+      </c>
+      <c r="AB18" t="s" s="5">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="6"/>
+      <c r="B19" t="s" s="5">
+        <v>462</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>463</v>
+      </c>
+      <c r="D19" t="s" s="5">
+        <v>464</v>
+      </c>
+      <c r="E19" t="s" s="5">
+        <v>465</v>
+      </c>
+      <c r="F19" t="s" s="5">
+        <v>466</v>
+      </c>
+      <c r="G19" t="s" s="5">
+        <v>467</v>
+      </c>
+      <c r="I19" t="s" s="5">
+        <v>552</v>
+      </c>
+      <c r="J19" t="s" s="5">
+        <v>553</v>
+      </c>
+      <c r="K19" t="s" s="5">
+        <v>554</v>
+      </c>
+      <c r="L19" t="s" s="5">
+        <v>555</v>
+      </c>
+      <c r="M19" t="s" s="5">
+        <v>556</v>
+      </c>
+      <c r="N19" t="s" s="5">
+        <v>557</v>
+      </c>
+      <c r="P19" t="s" s="5">
+        <v>642</v>
+      </c>
+      <c r="Q19" t="s" s="5">
+        <v>643</v>
+      </c>
+      <c r="R19" t="s" s="5">
+        <v>644</v>
+      </c>
+      <c r="S19" t="s" s="5">
+        <v>645</v>
+      </c>
+      <c r="T19" t="s" s="5">
+        <v>646</v>
+      </c>
+      <c r="U19" t="s" s="5">
+        <v>647</v>
+      </c>
+      <c r="W19" t="s" s="5">
+        <v>732</v>
+      </c>
+      <c r="X19" t="s" s="5">
+        <v>733</v>
+      </c>
+      <c r="Y19" t="s" s="5">
+        <v>734</v>
+      </c>
+      <c r="Z19" t="s" s="5">
+        <v>735</v>
+      </c>
+      <c r="AA19" t="s" s="5">
+        <v>736</v>
+      </c>
+      <c r="AB19" t="s" s="5">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A14:A18"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>